<commit_message>
notes on default parameters
</commit_message>
<xml_diff>
--- a/CombBLAS/Applications/MCL-notes.xlsx
+++ b/CombBLAS/Applications/MCL-notes.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14920" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14520" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="perfromance" sheetId="2" r:id="rId1"/>
     <sheet name="bug" sheetId="4" r:id="rId2"/>
     <sheet name="flowchart" sheetId="5" r:id="rId3"/>
+    <sheet name="Default parameters" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>The load-imbalance might increase from one iteration to the next.</t>
   </si>
@@ -46,12 +47,207 @@
   <si>
     <t>The problem was with not freeing memory allocated in multiwaymerge</t>
   </si>
+  <si>
+    <r>
+      <t>-scheme</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;num&gt; (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>use a preset resource scheme</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">There are currently seven different resource schemes, indexed 1..7. High schemes result in more expensive computations that may possibly be more accurate. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The default scheme is 4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. When </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>mcl</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is done, it will give a grade (the so called </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>jury synopsis</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">) to the appropriateness of the scheme used. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A low grade does not necessarily imply that the resulting clustering is bad</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - but anyway, a low grade should be reason to try for a higher scheme.</t>
+    </r>
+  </si>
+  <si>
+    <t>MCL Option</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Where defined?</t>
+  </si>
+  <si>
+    <t>src/mcl/procinit.c</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">static int dir_scheme[7][4]
+=  
+   {  {  3000,  400,  500, 90 }
+   ,  {  4000,  500,  600, 90 }
+   ,  {  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>5000,  600,  700, 90</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> }
+   ,  {  6000,  700,  800, 90 }
+   ,  {  7000,  800,  900, 90 }
+   ,  { 10000, 1100, 1400, 90 }
+   ,  { 10000, 1200, 1600, 90 }
+   }  ;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>schemevalues (p, s,r,pct) (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>red is default</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) Note: the code actually uses 1/p and pct/100</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -87,6 +283,52 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -105,12 +347,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -124,10 +372,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2531,7 +2794,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD60"/>
     </sheetView>
   </sheetViews>
@@ -2610,4 +2873,59 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="3" max="3" width="73" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" customWidth="1"/>
+    <col min="5" max="5" width="51.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="30">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="7" customFormat="1" ht="157" customHeight="1">
+      <c r="A2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
slight changes in recovery logic after selection
</commit_message>
<xml_diff>
--- a/CombBLAS/Applications/MCL-notes.xlsx
+++ b/CombBLAS/Applications/MCL-notes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14520" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38900" windowHeight="24720" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="perfromance" sheetId="2" r:id="rId1"/>
@@ -772,8 +772,8 @@
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -783,7 +783,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10731500" y="3721100"/>
-          <a:ext cx="3086100" cy="1574800"/>
+          <a:ext cx="3086100" cy="1739900"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -819,18 +819,7 @@
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>n = nnz(v)</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1600" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>v = v + topK(w[w&lt;p], r-n)</a:t>
+            <a:t>v' = topK(w, r)</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -844,32 +833,57 @@
         <a:p>
           <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="en-US" sz="1600">
+            <a:rPr lang="en-US" sz="1600" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>OR</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1600">
+            <a:t>OR </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>v</a:t>
-          </a:r>
+            <a:t>n = nnz(v)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-US" sz="1600" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t> = topK(w, r)</a:t>
-          </a:r>
+            <a:t> u = topK(w[w&lt;p], r-n)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>v' = v + u </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1600" baseline="0">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
           <a:endParaRPr lang="en-US" sz="1600">
             <a:solidFill>
               <a:schemeClr val="tx1"/>
@@ -1175,14 +1189,14 @@
     <xdr:from>
       <xdr:col>17</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:colOff>698500</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1191,8 +1205,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14071600" y="7823200"/>
-          <a:ext cx="3086100" cy="1574800"/>
+          <a:off x="14071600" y="7658100"/>
+          <a:ext cx="3136900" cy="1905000"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -1223,28 +1237,17 @@
         <a:p>
           <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="en-US" sz="1600" baseline="0">
+            <a:rPr lang="nl-NL" sz="1600" b="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>n = nnz(v)</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1600" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>v = v + topK(v'[v'&gt;p], r-n)</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="en-US" sz="1600" baseline="0">
+            <a:t>v = topK(v', r)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1600" b="0" baseline="0">
             <a:solidFill>
               <a:schemeClr val="tx1"/>
             </a:solidFill>
@@ -1253,37 +1256,54 @@
         <a:p>
           <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="en-US" sz="1600">
+            <a:rPr lang="en-US" sz="1600" b="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>OR</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1600">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>v</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1600" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> = topK(v', r)</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1600">
+            <a:t>OR </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1600" b="1" baseline="0">
             <a:solidFill>
               <a:schemeClr val="tx1"/>
             </a:solidFill>
           </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>n = nnz(v)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> u = topK(v'[v'&gt;p], r-n)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>v = v + u</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1293,14 +1313,14 @@
     <xdr:from>
       <xdr:col>17</xdr:col>
       <xdr:colOff>50800</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>660400</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1309,7 +1329,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14084300" y="9804400"/>
+          <a:off x="14084300" y="10401300"/>
           <a:ext cx="3086100" cy="469900"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
@@ -1775,15 +1795,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>755650</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:colOff>768350</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>768350</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:colOff>781050</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1794,9 +1814,9 @@
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="15614650" y="9398000"/>
-          <a:ext cx="12700" cy="406400"/>
+        <a:xfrm flipH="1">
+          <a:off x="15627350" y="9563100"/>
+          <a:ext cx="12700" cy="838200"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2404,6 +2424,458 @@
             </a:rPr>
             <a:t>No</a:t>
           </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="31" name="Rounded Rectangle 30"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14300200" y="3797300"/>
+          <a:ext cx="7061200" cy="1917700"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln w="28575" cmpd="sng">
+          <a:noFill/>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600">
+              <a:ln>
+                <a:noFill/>
+                <a:prstDash val="dot"/>
+              </a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+            </a:rPr>
+            <a:t>These</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" baseline="0">
+              <a:ln>
+                <a:noFill/>
+                <a:prstDash val="dot"/>
+              </a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+            </a:rPr>
+            <a:t> two options</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600">
+              <a:ln>
+                <a:noFill/>
+                <a:prstDash val="dot"/>
+              </a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+            </a:rPr>
+            <a:t> essentially produce</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" baseline="0">
+              <a:ln>
+                <a:noFill/>
+                <a:prstDash val="dot"/>
+              </a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+            </a:rPr>
+            <a:t> the same output. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" baseline="0">
+              <a:ln>
+                <a:noFill/>
+                <a:prstDash val="dot"/>
+              </a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+            </a:rPr>
+            <a:t>The first option keeps top r entries from the original vector w.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" baseline="0">
+              <a:ln>
+                <a:noFill/>
+                <a:prstDash val="dot"/>
+              </a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+            </a:rPr>
+            <a:t>The second option creates u by keeping top (r-n) entries from w \setminus v.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" baseline="0">
+              <a:ln>
+                <a:noFill/>
+                <a:prstDash val="dot"/>
+              </a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+            </a:rPr>
+            <a:t>u is then combined with v to get top r entries of the original vector w.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" baseline="0">
+              <a:ln>
+                <a:noFill/>
+                <a:prstDash val="dot"/>
+              </a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+            </a:rPr>
+            <a:t>The second option might be more efficient (topK computation is cheaper). </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" baseline="0">
+              <a:ln>
+                <a:noFill/>
+                <a:prstDash val="dot"/>
+              </a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+            </a:rPr>
+            <a:t>At this moment we have only implemented option 1.   </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1600">
+            <a:ln>
+              <a:noFill/>
+              <a:prstDash val="dot"/>
+            </a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>539750</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="34" name="Straight Arrow Connector 33"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7962900" y="7797800"/>
+          <a:ext cx="6350" cy="546100"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="36" name="Rounded Rectangle 35"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8191500" y="5562600"/>
+          <a:ext cx="1054100" cy="406400"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln w="28575" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" b="1">
+              <a:solidFill>
+                <a:srgbClr val="0000FF"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>No</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>558800</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>787400</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="39" name="Rounded Rectangle 38"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7988300" y="7874000"/>
+          <a:ext cx="1054100" cy="406400"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln w="28575" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="2000" b="1">
+              <a:solidFill>
+                <a:srgbClr val="0000FF"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>No</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="40" name="Rounded Rectangle 39"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6362700" y="8369300"/>
+          <a:ext cx="3086100" cy="469900"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="0000FF">
+            <a:alpha val="6000"/>
+          </a:srgbClr>
+        </a:solidFill>
+        <a:ln w="28575" cmpd="sng"/>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>return v</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1600">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -2779,7 +3251,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="38.6640625" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2817,7 +3289,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:XFD60"/>
     </sheetView>
   </sheetViews>
@@ -2902,7 +3374,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
MCL loop adjustment added and column-by-column decision of recovery/seelct logic added
</commit_message>
<xml_diff>
--- a/CombBLAS/Applications/MCL-notes.xlsx
+++ b/CombBLAS/Applications/MCL-notes.xlsx
@@ -4,13 +4,16 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38900" windowHeight="24720" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14720" tabRatio="500" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="perfromance" sheetId="2" r:id="rId1"/>
     <sheet name="bug" sheetId="4" r:id="rId2"/>
     <sheet name="flowchart" sheetId="5" r:id="rId3"/>
     <sheet name="Default parameters" sheetId="6" r:id="rId4"/>
+    <sheet name="mcl calls" sheetId="7" r:id="rId5"/>
+    <sheet name="Loops" sheetId="8" r:id="rId6"/>
+    <sheet name="cage4- example (manuasymmetric)" sheetId="10" r:id="rId7"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="60">
   <si>
     <t>The load-imbalance might increase from one iteration to the next.</t>
   </si>
@@ -260,12 +263,164 @@
    }  ;</t>
     </r>
   </si>
+  <si>
+    <t>mclAlgorithmStart (alg.c)</t>
+  </si>
+  <si>
+    <t>mclxIOstreamIn(Impala/stream.c)</t>
+  </si>
+  <si>
+    <t>1. read raw file by =&gt;</t>
+  </si>
+  <si>
+    <t>mclAlgorithmTransform</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>--discard-loops=y</t>
+  </si>
+  <si>
+    <t>mcl option</t>
+  </si>
+  <si>
+    <t>action</t>
+  </si>
+  <si>
+    <t>--sum-loops</t>
+  </si>
+  <si>
+    <t>--discard-loops=f</t>
+  </si>
+  <si>
+    <t>set loops to max of all arc weights (including the initial loop)</t>
+  </si>
+  <si>
+    <t>set loops to sum of other arcs weights (excluding the initial loop)</t>
+  </si>
+  <si>
+    <t>remove all loops and then add set loops to max of all arc weights (essentially set loops to max of all arc weights excluding the initial loops)</t>
+  </si>
+  <si>
+    <t>function mclAlgorithmTransform in alg.c file</t>
+  </si>
+  <si>
+    <t>2. Adjust loops (see Loops tab)</t>
+  </si>
+  <si>
+    <t>mclAlgorithmStreamIn(alg.c) =&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">in all cases: Add a loop with weight =1 for isolated vertices </t>
+  </si>
+  <si>
+    <t>3. Make Stochastic</t>
+  </si>
+  <si>
+    <t>mclxMakeStochastic</t>
+  </si>
+  <si>
+    <t>mclAlgorithm (alg.c)</t>
+  </si>
+  <si>
+    <t>1. preprocess data =&gt;</t>
+  </si>
+  <si>
+    <t>mclProcess (proc.c)</t>
+  </si>
+  <si>
+    <t>2. Other processing =&gt;</t>
+  </si>
+  <si>
+    <t>1. do iterations =&gt;</t>
+  </si>
+  <si>
+    <t>3. kselect?? (line 209)</t>
+  </si>
+  <si>
+    <t>doIteration (proc.c) [one iteration]</t>
+  </si>
+  <si>
+    <t>1. Expand =&gt;</t>
+  </si>
+  <si>
+    <t>2. Prune / hardthreasholding</t>
+  </si>
+  <si>
+    <t>3.2. overdid , threshold too small, recover</t>
+  </si>
+  <si>
+    <t>3.1. Add a loop if a column becomes empty</t>
+  </si>
+  <si>
+    <t>[</t>
+  </si>
+  <si>
+    <t>]</t>
+  </si>
+  <si>
+    <t>1. SpMSpV</t>
+  </si>
+  <si>
+    <t>mclExpand (expand.c) (for each column vector)</t>
+  </si>
+  <si>
+    <t>4.  normalize =&gt;</t>
+  </si>
+  <si>
+    <t>mclvNormalize or mclvScale  (impala/vector.c)</t>
+  </si>
+  <si>
+    <t>3.3. threshold too large, reduce further, select =&gt;</t>
+  </si>
+  <si>
+    <t>see 3.3 below</t>
+  </si>
+  <si>
+    <t>5. compute chaos</t>
+  </si>
+  <si>
+    <t>Note: there is a mismatch in chaos computation based on  --partition-selection option. If  --partition-selection option is used mclExpandVector2 function is called. Otherwise mclExpandVector1 funciton is called. mclExpandVector2 calculate sum of square and maximum value immediately after multiplication before pruning/recovery/selection. By contrast, mclExpandVector2 calculate these number after pruning/recovery/selection. Hence, the cahos returned by these two functions are different. mclExpandVector2 makes more sense to me and it matches to our code. This issue is reported to mcl-users@ebi.ac.uk</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">either mclvKBar/mclvSelectGqBar (heap-based kselect when </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>--partition-selection</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> option not used) or selectk (partition based kselect when --partition-selection option is used) (impala/vector.c)</t>
+    </r>
+  </si>
+  <si>
+    <t>2. Inflate =&gt;</t>
+  </si>
+  <si>
+    <t>Inflate and normalize</t>
+  </si>
+  <si>
+    <t>2. Make Stochastic (why again?)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -352,13 +507,38 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -370,7 +550,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -380,8 +560,36 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -404,16 +612,63 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="37">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3289,7 +3544,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD60"/>
     </sheetView>
   </sheetViews>
@@ -3375,7 +3630,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3423,4 +3678,1751 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:F22"/>
+  <sheetViews>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="23" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="8"/>
+    <col min="2" max="2" width="37.5" style="8" customWidth="1"/>
+    <col min="3" max="3" width="48" style="8" customWidth="1"/>
+    <col min="4" max="4" width="40.33203125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="66.6640625" style="8" customWidth="1"/>
+    <col min="6" max="6" width="59.33203125" style="8" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:6">
+      <c r="B4" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="B5" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="C6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6">
+      <c r="C7" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6">
+      <c r="C8" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6">
+      <c r="B10" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6">
+      <c r="C11" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6">
+      <c r="D12" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6">
+      <c r="E13" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6">
+      <c r="E14" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6">
+      <c r="E15" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6">
+      <c r="E16" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" ht="115">
+      <c r="E17" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6">
+      <c r="E18" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="3:6" ht="345">
+      <c r="E19" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6">
+      <c r="D20" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="3:6">
+      <c r="C21" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="3:6">
+      <c r="C22" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H43"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="2" width="29.33203125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="65" style="9" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="30">
+      <c r="B1" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="B2" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="30">
+      <c r="A3" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="B4" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="B5" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="30">
+      <c r="B9" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" spans="8:8" ht="23">
+      <c r="H43" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D2:W25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="O31" sqref="O31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="2" spans="4:23">
+      <c r="D2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2">
+        <v>0.189</v>
+      </c>
+      <c r="F2">
+        <v>0.108</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2" t="s">
+        <v>47</v>
+      </c>
+      <c r="O2">
+        <v>0.19</v>
+      </c>
+      <c r="P2">
+        <v>0.11</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0.1</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0.06</v>
+      </c>
+      <c r="W2">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="3" spans="4:23">
+      <c r="D3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3">
+        <v>0.11600000000000001</v>
+      </c>
+      <c r="F3">
+        <v>0.21199999999999999</v>
+      </c>
+      <c r="G3">
+        <v>0.191</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>6.3E-2</v>
+      </c>
+      <c r="J3">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3" t="s">
+        <v>47</v>
+      </c>
+      <c r="O3">
+        <v>0.12</v>
+      </c>
+      <c r="P3">
+        <v>0.21</v>
+      </c>
+      <c r="Q3">
+        <v>0.19</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>0.06</v>
+      </c>
+      <c r="T3">
+        <v>0.09</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="4" spans="4:23">
+      <c r="D4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="G4">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4" t="s">
+        <v>47</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0.08</v>
+      </c>
+      <c r="Q4">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="4:23">
+      <c r="D5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0.155</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="L5">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5" t="s">
+        <v>47</v>
+      </c>
+      <c r="O5">
+        <v>0.09</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0.16</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="V5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="W5">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="6" spans="4:23">
+      <c r="D6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6">
+        <v>0.214</v>
+      </c>
+      <c r="F6">
+        <v>0.252</v>
+      </c>
+      <c r="G6">
+        <v>0.189</v>
+      </c>
+      <c r="H6">
+        <v>0.109</v>
+      </c>
+      <c r="I6">
+        <v>0.254</v>
+      </c>
+      <c r="J6">
+        <v>0.23799999999999999</v>
+      </c>
+      <c r="K6">
+        <v>0.17299999999999999</v>
+      </c>
+      <c r="L6">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="M6">
+        <v>0.222</v>
+      </c>
+      <c r="N6" t="s">
+        <v>47</v>
+      </c>
+      <c r="O6">
+        <v>0.21</v>
+      </c>
+      <c r="P6">
+        <v>0.25</v>
+      </c>
+      <c r="Q6">
+        <v>0.19</v>
+      </c>
+      <c r="R6">
+        <v>0.11</v>
+      </c>
+      <c r="S6">
+        <v>0.25</v>
+      </c>
+      <c r="T6">
+        <v>0.24</v>
+      </c>
+      <c r="U6">
+        <v>0.17</v>
+      </c>
+      <c r="V6">
+        <v>0.17</v>
+      </c>
+      <c r="W6">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="4:23">
+      <c r="D7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="G7">
+        <v>0.182</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0.113</v>
+      </c>
+      <c r="J7">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="K7">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>9.4E-2</v>
+      </c>
+      <c r="N7" t="s">
+        <v>47</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0.17</v>
+      </c>
+      <c r="Q7">
+        <v>0.18</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>0.11</v>
+      </c>
+      <c r="T7">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="U7">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="8" spans="4:23">
+      <c r="D8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="H8">
+        <v>0.191</v>
+      </c>
+      <c r="I8">
+        <v>0.11</v>
+      </c>
+      <c r="J8">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="K8">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="L8">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="M8">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="N8" t="s">
+        <v>47</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0.15</v>
+      </c>
+      <c r="R8">
+        <v>0.19</v>
+      </c>
+      <c r="S8">
+        <v>0.11</v>
+      </c>
+      <c r="T8">
+        <v>0.1</v>
+      </c>
+      <c r="U8">
+        <v>0.17</v>
+      </c>
+      <c r="V8">
+        <v>0.15</v>
+      </c>
+      <c r="W8">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="9" spans="4:23">
+      <c r="D9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0.222</v>
+      </c>
+      <c r="I9">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="J9">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="K9">
+        <v>0.19800000000000001</v>
+      </c>
+      <c r="L9">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="M9">
+        <v>0.19</v>
+      </c>
+      <c r="N9" t="s">
+        <v>47</v>
+      </c>
+      <c r="O9">
+        <v>0.18</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>0.22</v>
+      </c>
+      <c r="S9">
+        <v>0.15</v>
+      </c>
+      <c r="T9">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="U9">
+        <v>0.2</v>
+      </c>
+      <c r="V9">
+        <v>0.23</v>
+      </c>
+      <c r="W9">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="10" spans="4:23">
+      <c r="D10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10">
+        <v>0.219</v>
+      </c>
+      <c r="F10">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="G10">
+        <v>0.156</v>
+      </c>
+      <c r="H10">
+        <v>0.223</v>
+      </c>
+      <c r="I10">
+        <v>0.312</v>
+      </c>
+      <c r="J10">
+        <v>0.29899999999999999</v>
+      </c>
+      <c r="K10">
+        <v>0.309</v>
+      </c>
+      <c r="L10">
+        <v>0.316</v>
+      </c>
+      <c r="M10">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="N10" t="s">
+        <v>47</v>
+      </c>
+      <c r="O10">
+        <v>0.22</v>
+      </c>
+      <c r="P10">
+        <v>0.17</v>
+      </c>
+      <c r="Q10">
+        <v>0.16</v>
+      </c>
+      <c r="R10">
+        <v>0.22</v>
+      </c>
+      <c r="S10">
+        <v>0.31</v>
+      </c>
+      <c r="T10">
+        <v>0.3</v>
+      </c>
+      <c r="U10">
+        <v>0.31</v>
+      </c>
+      <c r="V10">
+        <v>0.32</v>
+      </c>
+      <c r="W10">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="12" spans="4:23">
+      <c r="E12">
+        <f>E2^2</f>
+        <v>3.5721000000000003E-2</v>
+      </c>
+      <c r="F12">
+        <f t="shared" ref="F12:W12" si="0">F2^2</f>
+        <v>1.1663999999999999E-2</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>9.8010000000000007E-3</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>3.4809999999999997E-3</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N12" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="0"/>
+        <v>3.61E-2</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="0"/>
+        <v>1.21E-2</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000002E-2</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V12">
+        <f t="shared" si="0"/>
+        <v>3.5999999999999999E-3</v>
+      </c>
+      <c r="W12">
+        <f t="shared" si="0"/>
+        <v>8.9999999999999998E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="4:23">
+      <c r="E13">
+        <f t="shared" ref="E13:W13" si="1">E3^2</f>
+        <v>1.3456000000000001E-2</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>4.4943999999999998E-2</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>3.6481E-2</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="1"/>
+        <v>3.9690000000000003E-3</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="1"/>
+        <v>7.5689999999999993E-3</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N13" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="1"/>
+        <v>1.44E-2</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="1"/>
+        <v>4.4099999999999993E-2</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="1"/>
+        <v>3.61E-2</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <f t="shared" si="1"/>
+        <v>3.5999999999999999E-3</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="1"/>
+        <v>8.0999999999999996E-3</v>
+      </c>
+      <c r="U13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="V13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="W13">
+        <f t="shared" si="1"/>
+        <v>8.9999999999999998E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="4:23">
+      <c r="E14">
+        <f t="shared" ref="E14:W14" si="2">E4^2</f>
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="2"/>
+        <v>6.889000000000001E-3</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="2"/>
+        <v>1.8496000000000002E-2</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N14" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="2"/>
+        <v>6.4000000000000003E-3</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="2"/>
+        <v>1.9600000000000003E-2</v>
+      </c>
+      <c r="R14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="V14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="W14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="4:23">
+      <c r="E15">
+        <f t="shared" ref="E15:W15" si="3">E5^2</f>
+        <v>7.3959999999999989E-3</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="3"/>
+        <v>2.4025000000000001E-2</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="3"/>
+        <v>5.6249999999999998E-3</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="3"/>
+        <v>4.7610000000000005E-3</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="N15" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="3"/>
+        <v>8.0999999999999996E-3</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <f t="shared" si="3"/>
+        <v>2.5600000000000001E-2</v>
+      </c>
+      <c r="S15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U15">
+        <f t="shared" si="3"/>
+        <v>4.9000000000000007E-3</v>
+      </c>
+      <c r="V15">
+        <f t="shared" si="3"/>
+        <v>4.9000000000000007E-3</v>
+      </c>
+      <c r="W15">
+        <f t="shared" si="3"/>
+        <v>8.9999999999999998E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="4:23">
+      <c r="E16">
+        <f t="shared" ref="E16:W16" si="4">E6^2</f>
+        <v>4.5795999999999996E-2</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="4"/>
+        <v>6.3504000000000005E-2</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="4"/>
+        <v>3.5721000000000003E-2</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="4"/>
+        <v>1.1880999999999999E-2</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="4"/>
+        <v>6.4516000000000004E-2</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="4"/>
+        <v>5.6643999999999993E-2</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="4"/>
+        <v>2.9928999999999997E-2</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="4"/>
+        <v>3.0624999999999996E-2</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="4"/>
+        <v>4.9284000000000001E-2</v>
+      </c>
+      <c r="N16" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="4"/>
+        <v>4.4099999999999993E-2</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="4"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" si="4"/>
+        <v>3.61E-2</v>
+      </c>
+      <c r="R16">
+        <f t="shared" si="4"/>
+        <v>1.21E-2</v>
+      </c>
+      <c r="S16">
+        <f t="shared" si="4"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="4"/>
+        <v>5.7599999999999998E-2</v>
+      </c>
+      <c r="U16">
+        <f t="shared" si="4"/>
+        <v>2.8900000000000006E-2</v>
+      </c>
+      <c r="V16">
+        <f t="shared" si="4"/>
+        <v>2.8900000000000006E-2</v>
+      </c>
+      <c r="W16">
+        <f t="shared" si="4"/>
+        <v>4.0000000000000008E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="5:23">
+      <c r="E17">
+        <f t="shared" ref="E17:W17" si="5">E7^2</f>
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="5"/>
+        <v>2.9241000000000003E-2</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="5"/>
+        <v>3.3124000000000001E-2</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="5"/>
+        <v>1.2769000000000001E-2</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="5"/>
+        <v>1.9044000000000002E-2</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="5"/>
+        <v>4.9000000000000007E-3</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="5"/>
+        <v>8.8360000000000001E-3</v>
+      </c>
+      <c r="N17" t="e">
+        <f t="shared" si="5"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="5"/>
+        <v>2.8900000000000006E-2</v>
+      </c>
+      <c r="Q17">
+        <f t="shared" si="5"/>
+        <v>3.2399999999999998E-2</v>
+      </c>
+      <c r="R17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <f t="shared" si="5"/>
+        <v>1.21E-2</v>
+      </c>
+      <c r="T17">
+        <f t="shared" si="5"/>
+        <v>1.9600000000000003E-2</v>
+      </c>
+      <c r="U17">
+        <f t="shared" si="5"/>
+        <v>4.9000000000000007E-3</v>
+      </c>
+      <c r="V17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="W17">
+        <f t="shared" si="5"/>
+        <v>8.0999999999999996E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="5:23">
+      <c r="E18">
+        <f t="shared" ref="E18:W18" si="6">E8^2</f>
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="6"/>
+        <v>2.1315999999999998E-2</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="6"/>
+        <v>3.6481E-2</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="6"/>
+        <v>1.21E-2</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="6"/>
+        <v>1.0403999999999998E-2</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="6"/>
+        <v>3.0624999999999996E-2</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="6"/>
+        <v>2.1608999999999996E-2</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="6"/>
+        <v>1.7956000000000003E-2</v>
+      </c>
+      <c r="N18" t="e">
+        <f t="shared" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <f t="shared" si="6"/>
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="R18">
+        <f t="shared" si="6"/>
+        <v>3.61E-2</v>
+      </c>
+      <c r="S18">
+        <f t="shared" si="6"/>
+        <v>1.21E-2</v>
+      </c>
+      <c r="T18">
+        <f t="shared" si="6"/>
+        <v>1.0000000000000002E-2</v>
+      </c>
+      <c r="U18">
+        <f t="shared" si="6"/>
+        <v>2.8900000000000006E-2</v>
+      </c>
+      <c r="V18">
+        <f t="shared" si="6"/>
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="W18">
+        <f t="shared" si="6"/>
+        <v>1.44E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="5:23">
+      <c r="E19">
+        <f t="shared" ref="E19:W19" si="7">E9^2</f>
+        <v>3.0975999999999997E-2</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="7"/>
+        <v>4.9284000000000001E-2</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="7"/>
+        <v>2.1903999999999996E-2</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="7"/>
+        <v>1.8496000000000002E-2</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="7"/>
+        <v>3.9204000000000003E-2</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="7"/>
+        <v>5.4756000000000006E-2</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="7"/>
+        <v>3.61E-2</v>
+      </c>
+      <c r="N19" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="7"/>
+        <v>3.2399999999999998E-2</v>
+      </c>
+      <c r="P19">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="R19">
+        <f t="shared" si="7"/>
+        <v>4.8399999999999999E-2</v>
+      </c>
+      <c r="S19">
+        <f t="shared" si="7"/>
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="T19">
+        <f t="shared" si="7"/>
+        <v>1.9600000000000003E-2</v>
+      </c>
+      <c r="U19">
+        <f t="shared" si="7"/>
+        <v>4.0000000000000008E-2</v>
+      </c>
+      <c r="V19">
+        <f t="shared" si="7"/>
+        <v>5.2900000000000003E-2</v>
+      </c>
+      <c r="W19">
+        <f t="shared" si="7"/>
+        <v>2.8900000000000006E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="5:23">
+      <c r="E20">
+        <f t="shared" ref="E20:W20" si="8">E10^2</f>
+        <v>4.7960999999999997E-2</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="8"/>
+        <v>3.0624999999999996E-2</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="8"/>
+        <v>2.4336E-2</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="8"/>
+        <v>4.9729000000000002E-2</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="8"/>
+        <v>9.7344E-2</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="8"/>
+        <v>8.9400999999999994E-2</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="8"/>
+        <v>9.5480999999999996E-2</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="8"/>
+        <v>9.9856E-2</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="8"/>
+        <v>0.13032099999999999</v>
+      </c>
+      <c r="N20" t="e">
+        <f t="shared" si="8"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="8"/>
+        <v>4.8399999999999999E-2</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="8"/>
+        <v>2.8900000000000006E-2</v>
+      </c>
+      <c r="Q20">
+        <f t="shared" si="8"/>
+        <v>2.5600000000000001E-2</v>
+      </c>
+      <c r="R20">
+        <f t="shared" si="8"/>
+        <v>4.8399999999999999E-2</v>
+      </c>
+      <c r="S20">
+        <f t="shared" si="8"/>
+        <v>9.6100000000000005E-2</v>
+      </c>
+      <c r="T20">
+        <f t="shared" si="8"/>
+        <v>0.09</v>
+      </c>
+      <c r="U20">
+        <f t="shared" si="8"/>
+        <v>9.6100000000000005E-2</v>
+      </c>
+      <c r="V20">
+        <f t="shared" si="8"/>
+        <v>0.1024</v>
+      </c>
+      <c r="W20">
+        <f t="shared" si="8"/>
+        <v>0.10890000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="5:23">
+      <c r="E22">
+        <f>SUM(E12:E20)</f>
+        <v>0.18130599999999999</v>
+      </c>
+      <c r="F22">
+        <f t="shared" ref="F22:W22" si="9">SUM(F12:F20)</f>
+        <v>0.18686699999999998</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="9"/>
+        <v>0.16947399999999999</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="9"/>
+        <v>0.181201</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="9"/>
+        <v>0.21260200000000001</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="9"/>
+        <v>0.20155799999999999</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="9"/>
+        <v>0.205764</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="9"/>
+        <v>0.215088</v>
+      </c>
+      <c r="M22">
+        <f t="shared" si="9"/>
+        <v>0.24249699999999999</v>
+      </c>
+      <c r="N22" t="e">
+        <f t="shared" si="9"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O22">
+        <f t="shared" si="9"/>
+        <v>0.1835</v>
+      </c>
+      <c r="P22">
+        <f t="shared" si="9"/>
+        <v>0.18290000000000001</v>
+      </c>
+      <c r="Q22">
+        <f t="shared" si="9"/>
+        <v>0.17230000000000001</v>
+      </c>
+      <c r="R22">
+        <f t="shared" si="9"/>
+        <v>0.18060000000000001</v>
+      </c>
+      <c r="S22">
+        <f t="shared" si="9"/>
+        <v>0.20890000000000003</v>
+      </c>
+      <c r="T22">
+        <f t="shared" si="9"/>
+        <v>0.2049</v>
+      </c>
+      <c r="U22">
+        <f t="shared" si="9"/>
+        <v>0.20370000000000002</v>
+      </c>
+      <c r="V22">
+        <f t="shared" si="9"/>
+        <v>0.2152</v>
+      </c>
+      <c r="W22">
+        <f t="shared" si="9"/>
+        <v>0.20300000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="5:23">
+      <c r="E23">
+        <f>MAX(E2:E10)</f>
+        <v>0.219</v>
+      </c>
+      <c r="F23">
+        <f t="shared" ref="F23:W23" si="10">MAX(F2:F10)</f>
+        <v>0.252</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="10"/>
+        <v>0.191</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="10"/>
+        <v>0.223</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="10"/>
+        <v>0.312</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="10"/>
+        <v>0.29899999999999999</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="10"/>
+        <v>0.309</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="10"/>
+        <v>0.316</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="10"/>
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="10"/>
+        <v>0.22</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="10"/>
+        <v>0.25</v>
+      </c>
+      <c r="Q23">
+        <f t="shared" si="10"/>
+        <v>0.19</v>
+      </c>
+      <c r="R23">
+        <f t="shared" si="10"/>
+        <v>0.22</v>
+      </c>
+      <c r="S23">
+        <f t="shared" si="10"/>
+        <v>0.31</v>
+      </c>
+      <c r="T23">
+        <f t="shared" si="10"/>
+        <v>0.3</v>
+      </c>
+      <c r="U23">
+        <f t="shared" si="10"/>
+        <v>0.31</v>
+      </c>
+      <c r="V23">
+        <f t="shared" si="10"/>
+        <v>0.32</v>
+      </c>
+      <c r="W23">
+        <f t="shared" si="10"/>
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="25" spans="5:23">
+      <c r="E25">
+        <f>(E23-E22)*6</f>
+        <v>0.22616400000000003</v>
+      </c>
+      <c r="F25">
+        <f t="shared" ref="F25:W25" si="11">(F23-F22)*6</f>
+        <v>0.39079800000000015</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="11"/>
+        <v>0.1291560000000001</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="11"/>
+        <v>0.25079400000000002</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="11"/>
+        <v>0.59638799999999992</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="11"/>
+        <v>0.58465199999999995</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="11"/>
+        <v>0.61941599999999997</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="11"/>
+        <v>0.60547200000000001</v>
+      </c>
+      <c r="M25">
+        <f>(M23-M22)*5</f>
+        <v>0.59251500000000001</v>
+      </c>
+      <c r="N25" t="e">
+        <f t="shared" si="11"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="11"/>
+        <v>0.21900000000000003</v>
+      </c>
+      <c r="P25">
+        <f t="shared" si="11"/>
+        <v>0.40259999999999996</v>
+      </c>
+      <c r="Q25">
+        <f t="shared" si="11"/>
+        <v>0.10619999999999996</v>
+      </c>
+      <c r="R25">
+        <f t="shared" si="11"/>
+        <v>0.23639999999999994</v>
+      </c>
+      <c r="S25">
+        <f t="shared" si="11"/>
+        <v>0.60659999999999981</v>
+      </c>
+      <c r="T25">
+        <f t="shared" si="11"/>
+        <v>0.5706</v>
+      </c>
+      <c r="U25">
+        <f t="shared" si="11"/>
+        <v>0.63779999999999992</v>
+      </c>
+      <c r="V25">
+        <f t="shared" si="11"/>
+        <v>0.62880000000000003</v>
+      </c>
+      <c r="W25">
+        <f>(W23-W22)*8</f>
+        <v>1.016</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
combined logic of prune-select-recovery
</commit_message>
<xml_diff>
--- a/CombBLAS/Applications/MCL-notes.xlsx
+++ b/CombBLAS/Applications/MCL-notes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14720" tabRatio="500" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14700" tabRatio="500" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="perfromance" sheetId="2" r:id="rId1"/>
@@ -609,9 +609,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -630,6 +627,9 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="37">
@@ -1225,7 +1225,7 @@
                 <a:srgbClr val="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>nnz(v) &lt; s</a:t>
+            <a:t>nnz(v) &gt; s</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1800" baseline="0">
@@ -3544,72 +3544,72 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:XFD60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" s="7" customFormat="1"/>
-    <row r="2" s="7" customFormat="1"/>
-    <row r="3" s="7" customFormat="1"/>
-    <row r="4" s="7" customFormat="1"/>
-    <row r="5" s="7" customFormat="1"/>
-    <row r="6" s="7" customFormat="1"/>
-    <row r="7" s="7" customFormat="1"/>
-    <row r="8" s="7" customFormat="1"/>
-    <row r="9" s="7" customFormat="1"/>
-    <row r="10" s="7" customFormat="1"/>
-    <row r="11" s="7" customFormat="1"/>
-    <row r="12" s="7" customFormat="1"/>
-    <row r="13" s="7" customFormat="1"/>
-    <row r="14" s="7" customFormat="1"/>
-    <row r="15" s="7" customFormat="1"/>
-    <row r="16" s="7" customFormat="1"/>
-    <row r="17" s="7" customFormat="1"/>
-    <row r="18" s="7" customFormat="1"/>
-    <row r="19" s="7" customFormat="1"/>
-    <row r="20" s="7" customFormat="1"/>
-    <row r="21" s="7" customFormat="1"/>
-    <row r="22" s="7" customFormat="1"/>
-    <row r="23" s="7" customFormat="1"/>
-    <row r="24" s="7" customFormat="1"/>
-    <row r="25" s="7" customFormat="1"/>
-    <row r="26" s="7" customFormat="1"/>
-    <row r="27" s="7" customFormat="1"/>
-    <row r="28" s="7" customFormat="1"/>
-    <row r="29" s="7" customFormat="1"/>
-    <row r="30" s="7" customFormat="1"/>
-    <row r="31" s="7" customFormat="1"/>
-    <row r="32" s="7" customFormat="1"/>
-    <row r="33" s="7" customFormat="1"/>
-    <row r="34" s="7" customFormat="1"/>
-    <row r="35" s="7" customFormat="1"/>
-    <row r="36" s="7" customFormat="1"/>
-    <row r="37" s="7" customFormat="1"/>
-    <row r="38" s="7" customFormat="1"/>
-    <row r="39" s="7" customFormat="1"/>
-    <row r="40" s="7" customFormat="1"/>
-    <row r="41" s="7" customFormat="1"/>
-    <row r="42" s="7" customFormat="1"/>
-    <row r="43" s="7" customFormat="1"/>
-    <row r="44" s="7" customFormat="1"/>
-    <row r="45" s="7" customFormat="1"/>
-    <row r="46" s="7" customFormat="1"/>
-    <row r="47" s="7" customFormat="1"/>
-    <row r="48" s="7" customFormat="1"/>
-    <row r="49" s="7" customFormat="1"/>
-    <row r="50" s="7" customFormat="1"/>
-    <row r="51" s="7" customFormat="1"/>
-    <row r="52" s="7" customFormat="1"/>
-    <row r="53" s="7" customFormat="1"/>
-    <row r="54" s="7" customFormat="1"/>
-    <row r="55" s="7" customFormat="1"/>
-    <row r="56" s="7" customFormat="1"/>
-    <row r="57" s="7" customFormat="1"/>
-    <row r="58" s="7" customFormat="1"/>
-    <row r="59" s="7" customFormat="1"/>
-    <row r="60" s="7" customFormat="1"/>
+    <row r="1" s="14" customFormat="1"/>
+    <row r="2" s="14" customFormat="1"/>
+    <row r="3" s="14" customFormat="1"/>
+    <row r="4" s="14" customFormat="1"/>
+    <row r="5" s="14" customFormat="1"/>
+    <row r="6" s="14" customFormat="1"/>
+    <row r="7" s="14" customFormat="1"/>
+    <row r="8" s="14" customFormat="1"/>
+    <row r="9" s="14" customFormat="1"/>
+    <row r="10" s="14" customFormat="1"/>
+    <row r="11" s="14" customFormat="1"/>
+    <row r="12" s="14" customFormat="1"/>
+    <row r="13" s="14" customFormat="1"/>
+    <row r="14" s="14" customFormat="1"/>
+    <row r="15" s="14" customFormat="1"/>
+    <row r="16" s="14" customFormat="1"/>
+    <row r="17" s="14" customFormat="1"/>
+    <row r="18" s="14" customFormat="1"/>
+    <row r="19" s="14" customFormat="1"/>
+    <row r="20" s="14" customFormat="1"/>
+    <row r="21" s="14" customFormat="1"/>
+    <row r="22" s="14" customFormat="1"/>
+    <row r="23" s="14" customFormat="1"/>
+    <row r="24" s="14" customFormat="1"/>
+    <row r="25" s="14" customFormat="1"/>
+    <row r="26" s="14" customFormat="1"/>
+    <row r="27" s="14" customFormat="1"/>
+    <row r="28" s="14" customFormat="1"/>
+    <row r="29" s="14" customFormat="1"/>
+    <row r="30" s="14" customFormat="1"/>
+    <row r="31" s="14" customFormat="1"/>
+    <row r="32" s="14" customFormat="1"/>
+    <row r="33" s="14" customFormat="1"/>
+    <row r="34" s="14" customFormat="1"/>
+    <row r="35" s="14" customFormat="1"/>
+    <row r="36" s="14" customFormat="1"/>
+    <row r="37" s="14" customFormat="1"/>
+    <row r="38" s="14" customFormat="1"/>
+    <row r="39" s="14" customFormat="1"/>
+    <row r="40" s="14" customFormat="1"/>
+    <row r="41" s="14" customFormat="1"/>
+    <row r="42" s="14" customFormat="1"/>
+    <row r="43" s="14" customFormat="1"/>
+    <row r="44" s="14" customFormat="1"/>
+    <row r="45" s="14" customFormat="1"/>
+    <row r="46" s="14" customFormat="1"/>
+    <row r="47" s="14" customFormat="1"/>
+    <row r="48" s="14" customFormat="1"/>
+    <row r="49" s="14" customFormat="1"/>
+    <row r="50" s="14" customFormat="1"/>
+    <row r="51" s="14" customFormat="1"/>
+    <row r="52" s="14" customFormat="1"/>
+    <row r="53" s="14" customFormat="1"/>
+    <row r="54" s="14" customFormat="1"/>
+    <row r="55" s="14" customFormat="1"/>
+    <row r="56" s="14" customFormat="1"/>
+    <row r="57" s="14" customFormat="1"/>
+    <row r="58" s="14" customFormat="1"/>
+    <row r="59" s="14" customFormat="1"/>
+    <row r="60" s="14" customFormat="1"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:XFD60"/>
@@ -3684,147 +3684,147 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:F22"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="23" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="8"/>
-    <col min="2" max="2" width="37.5" style="8" customWidth="1"/>
-    <col min="3" max="3" width="48" style="8" customWidth="1"/>
-    <col min="4" max="4" width="40.33203125" style="8" customWidth="1"/>
-    <col min="5" max="5" width="66.6640625" style="8" customWidth="1"/>
-    <col min="6" max="6" width="59.33203125" style="8" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="8"/>
+    <col min="1" max="1" width="10.83203125" style="7"/>
+    <col min="2" max="2" width="37.5" style="7" customWidth="1"/>
+    <col min="3" max="3" width="48" style="7" customWidth="1"/>
+    <col min="4" max="4" width="40.33203125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="66.6640625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="59.33203125" style="7" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:6">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="5" spans="2:6">
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="6" spans="2:6">
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="7" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="7" spans="2:6">
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="7" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="8" spans="2:6">
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="7" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="10" spans="2:6">
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="11" spans="2:6">
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="7" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="12" spans="2:6">
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="7" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="13" spans="2:6">
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="7" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="14" spans="2:6">
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="7" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="15" spans="2:6">
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="7" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="16" spans="2:6">
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="F16" s="7" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="17" spans="3:6" ht="115">
-      <c r="E17" s="8" t="s">
+      <c r="E17" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="F17" s="13" t="s">
+      <c r="F17" s="12" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="18" spans="3:6">
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="F18" s="8" t="s">
+      <c r="F18" s="7" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="19" spans="3:6" ht="345">
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="F19" s="14" t="s">
+      <c r="F19" s="13" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="20" spans="3:6">
-      <c r="D20" s="8" t="s">
+      <c r="D20" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E20" s="7" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="21" spans="3:6">
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="7" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="22" spans="3:6">
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="7" t="s">
         <v>40</v>
       </c>
     </row>
@@ -3849,58 +3849,58 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="2" width="29.33203125" style="9" customWidth="1"/>
-    <col min="3" max="3" width="65" style="9" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="9"/>
+    <col min="1" max="2" width="29.33203125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="65" style="8" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="30">
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="30">
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="43" spans="8:8" ht="23">
-      <c r="H43" s="11"/>
+      <c r="H43" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3917,7 +3917,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D2:W25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="O31" sqref="O31"/>
     </sheetView>
   </sheetViews>
@@ -5345,7 +5345,7 @@
         <v>0.22616400000000003</v>
       </c>
       <c r="F25">
-        <f t="shared" ref="F25:W25" si="11">(F23-F22)*6</f>
+        <f t="shared" ref="F25:V25" si="11">(F23-F22)*6</f>
         <v>0.39079800000000015</v>
       </c>
       <c r="G25">

</xml_diff>

<commit_message>
more timing informaiton and multithreading inflation
</commit_message>
<xml_diff>
--- a/CombBLAS/Applications/MCL-notes.xlsx
+++ b/CombBLAS/Applications/MCL-notes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14640" tabRatio="500" firstSheet="3" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14640" tabRatio="500" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="perfromance" sheetId="2" r:id="rId1"/>
@@ -3719,8 +3719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:F22"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="D18" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="23" x14ac:dyDescent="0"/>
@@ -5466,7 +5466,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>

</xml_diff>